<commit_message>
Added the updated version of Supplemental Table 5.
</commit_message>
<xml_diff>
--- a/Analysis/Genomics_manuscript_TIR/Supplemental_Figures/Supplemental_Table_5.xlsx
+++ b/Analysis/Genomics_manuscript_TIR/Supplemental_Figures/Supplemental_Table_5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work_Files\GCMP_TIR\immunity_microbiome\Supplemental_Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDE7902-8FB3-4A9E-9555-919EEAFD745A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA6BFD5-C27E-4E3E-B06E-5DE18EC06217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3132" yWindow="1908" windowWidth="17280" windowHeight="8964" xr2:uid="{E26483DB-0F68-41D3-8636-C00A52BBB5E8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E26483DB-0F68-41D3-8636-C00A52BBB5E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Table S5A" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
   <si>
-    <t>Microbiome richness in all, mucus, tissue, and skeleton compartments.</t>
-  </si>
-  <si>
     <t>Species</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>POR_Porites_rus</t>
   </si>
   <si>
-    <t>Microbiome evenness in all, mucus, tissue, and skeleton compartments.</t>
-  </si>
-  <si>
     <t>gini_index</t>
   </si>
   <si>
@@ -96,16 +90,22 @@
     <t>N_samples</t>
   </si>
   <si>
-    <t>Table S5B</t>
-  </si>
-  <si>
     <t>obs_asvs</t>
   </si>
   <si>
     <t>ln_asvs</t>
   </si>
   <si>
-    <t>Table S5A</t>
+    <t>Table S5A: Microbiome richness in all, mucus, tissue, and skeleton compartments</t>
+  </si>
+  <si>
+    <t>Microbiome richness in all, mucus, tissue, and skeleton compartments calculated using Qiime 2 for the coral genome species used in this study.</t>
+  </si>
+  <si>
+    <t>Table S5B: Microbiome evenness in all, mucus, tissue and skeleton compartments</t>
+  </si>
+  <si>
+    <t>Microbiome evenness in all, mucus, tissue, and skeleton compartments as calculated using QIIME2 for the coral species used in this study.</t>
   </si>
 </sst>
 </file>
@@ -226,36 +226,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -573,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CB40D2-B567-407D-9F11-E06022A77E50}">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -594,533 +597,551 @@
     <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
     </row>
     <row r="2" spans="1:13" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="7" t="s">
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5">
         <v>38</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>44.157894740000003</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>3.7879999999999998</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>16</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>50.25</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>3.9170105469999998</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="9">
         <v>12</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="9">
         <v>42.083333000000003</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="9">
         <v>3.7396517720000002</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="11">
         <v>10</v>
       </c>
-      <c r="L5" s="15">
+      <c r="L5" s="11">
         <v>30.6</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="11">
         <v>3.4210000090000001</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5">
         <v>10</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>37.299999999999997</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>3.6190000000000002</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>2</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>42</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <v>3.737669618</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="9">
         <v>4</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="9">
         <v>26.75</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="9">
         <v>3.2865344730000001</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="11">
         <v>4</v>
       </c>
-      <c r="L6" s="15">
+      <c r="L6" s="11">
         <v>44</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="11">
         <v>3.7841896340000001</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="6">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
         <v>37</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>78.918918919999996</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>4.3680000000000003</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>10</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <v>39.6</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <v>3.6788291179999999</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="9">
         <v>14</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="9">
         <v>80.357142859999996</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="9">
         <v>4.3864809850000004</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="11">
         <v>13</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="11">
         <v>98.307623000000007</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="11">
         <v>4.5881015720000002</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5">
+        <v>79</v>
+      </c>
+      <c r="D8" s="5">
+        <v>4.3689999999999998</v>
+      </c>
+      <c r="E8" s="7">
         <v>5</v>
       </c>
-      <c r="B8" s="6">
-        <v>15</v>
-      </c>
-      <c r="C8" s="6">
-        <v>79</v>
-      </c>
-      <c r="D8" s="6">
-        <v>4.3689999999999998</v>
-      </c>
-      <c r="E8" s="9">
-        <v>5</v>
-      </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>58.6</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <v>4.0707346969999998</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="9">
         <v>4</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="9">
         <v>86</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="9">
         <v>4.4543472959999999</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="11">
         <v>6</v>
       </c>
-      <c r="L8" s="15">
+      <c r="L8" s="11">
         <v>83.833330000000004</v>
       </c>
-      <c r="M8" s="15">
+      <c r="M8" s="11">
         <v>4.4288306610000001</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="6">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5">
         <v>9</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>88.555555560000002</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>4.484</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>2</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>58</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>4.0604430110000003</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="9">
         <v>3</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="9">
         <v>133.66667000000001</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="9">
         <v>4.8953491639999998</v>
       </c>
-      <c r="K9" s="15">
+      <c r="K9" s="11">
         <v>4</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="11">
         <v>65.75</v>
       </c>
-      <c r="M9" s="15">
+      <c r="M9" s="11">
         <v>4.1858596710000002</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5">
+        <v>25</v>
+      </c>
+      <c r="C10" s="5">
+        <v>69.12</v>
+      </c>
+      <c r="D10" s="5">
+        <v>4.2359999999999998</v>
+      </c>
+      <c r="E10" s="7">
         <v>7</v>
       </c>
-      <c r="B10" s="6">
-        <v>25</v>
-      </c>
-      <c r="C10" s="6">
-        <v>69.12</v>
-      </c>
-      <c r="D10" s="6">
-        <v>4.2359999999999998</v>
-      </c>
-      <c r="E10" s="9">
+      <c r="F10" s="7">
+        <v>90.857142999999994</v>
+      </c>
+      <c r="G10" s="7">
+        <v>4.5092884160000004</v>
+      </c>
+      <c r="H10" s="9">
         <v>7</v>
       </c>
-      <c r="F10" s="9">
-        <v>90.857142999999994</v>
-      </c>
-      <c r="G10" s="9">
-        <v>4.5092884160000004</v>
-      </c>
-      <c r="H10" s="12">
-        <v>7</v>
-      </c>
-      <c r="I10" s="12">
+      <c r="I10" s="9">
         <v>50.285710000000002</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="9">
         <v>3.9177209409999998</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="11">
         <v>11</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10" s="11">
         <v>68.363630000000001</v>
       </c>
-      <c r="M10" s="15">
+      <c r="M10" s="11">
         <v>4.2248409579999997</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5">
+        <v>193.69565220000001</v>
+      </c>
+      <c r="D11" s="5">
+        <v>5.266</v>
+      </c>
+      <c r="E11" s="7">
+        <v>9</v>
+      </c>
+      <c r="F11" s="7">
+        <v>75.111099999999993</v>
+      </c>
+      <c r="G11" s="7">
+        <v>4.3189683509999997</v>
+      </c>
+      <c r="H11" s="9">
         <v>8</v>
       </c>
-      <c r="B11" s="6">
-        <v>23</v>
-      </c>
-      <c r="C11" s="6">
-        <v>193.69565220000001</v>
-      </c>
-      <c r="D11" s="6">
-        <v>5.266</v>
-      </c>
-      <c r="E11" s="9">
-        <v>9</v>
-      </c>
-      <c r="F11" s="9">
-        <v>75.111099999999993</v>
-      </c>
-      <c r="G11" s="9">
-        <v>4.3189683509999997</v>
-      </c>
-      <c r="H11" s="12">
-        <v>8</v>
-      </c>
-      <c r="I11" s="12">
+      <c r="I11" s="9">
         <v>259.375</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="9">
         <v>5.5582748909999999</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="11">
         <v>6</v>
       </c>
-      <c r="L11" s="15">
+      <c r="L11" s="11">
         <v>269</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="11">
         <v>5.5947113799999997</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="6">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5">
         <v>2</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>55.5</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>4.016</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>1</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <v>44</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="7">
         <v>3.7841896340000001</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="9">
         <v>3</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="9">
         <v>64.332999999999998</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="9">
         <v>4.164072719</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="11">
         <v>1</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="11">
         <v>62</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="11">
         <v>4.1271343849999997</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="6">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5">
         <v>3</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>73.666669999999996</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>4.3</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="7">
         <v>1</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="7">
         <v>73</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="7">
         <v>4.2904594410000003</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="9">
         <v>1</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="9">
         <v>86</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="9">
         <v>4.4543472959999999</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="11">
         <v>1</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="11">
         <v>42</v>
       </c>
-      <c r="M13" s="15">
+      <c r="M13" s="11">
         <v>3.737669618</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="6">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5">
         <v>6</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>56.5</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>4.0339999999999998</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>3</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>48.333300000000001</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="7">
         <v>3.8781207640000002</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="9">
         <v>1</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="9">
         <v>28</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="9">
         <v>3.33220451</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="11">
         <v>2</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="11">
         <v>83</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="11">
         <v>4.418840608</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="6">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5">
         <v>15</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>114.266667</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>4.7389999999999999</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>5</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <v>74.400000000000006</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="7">
         <v>4.3094559419999996</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="9">
         <v>5</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="9">
         <v>85</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="9">
         <v>4.4426512560000004</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="11">
         <v>5</v>
       </c>
-      <c r="L15" s="15">
+      <c r="L15" s="11">
         <v>183.4</v>
       </c>
-      <c r="M15" s="15">
+      <c r="M15" s="11">
         <v>5.2116695599999998</v>
       </c>
     </row>
@@ -1130,8 +1151,8 @@
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="K3:M3"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1141,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD883FC-B09B-46FA-907D-7B0F8F7A09DA}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1160,385 +1181,393 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="7" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="13"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>14</v>
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5">
         <v>38</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>0.98045260000000001</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="7">
         <v>16</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>0.95429019999999998</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="9">
         <v>12</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="9">
         <v>0.95579400000000003</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="11">
         <v>10</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="11">
         <v>0.93784559999999995</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5">
         <v>10</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>0.9572117</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>2</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>0.83304299999999998</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="9">
         <v>4</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="9">
         <v>0.88848550000000004</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="11">
         <v>4</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="11">
         <v>0.92181716000000002</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="6">
+        <v>3</v>
+      </c>
+      <c r="B7" s="5">
         <v>37</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>0.98815768999999998</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="7">
         <v>10</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="7">
         <v>0.95153089999999996</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="9">
         <v>14</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="9">
         <v>0.97317739999999997</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="11">
         <v>13</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="11">
         <v>0.97013300000000002</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.97194899700000004</v>
+      </c>
+      <c r="D8" s="7">
         <v>5</v>
       </c>
-      <c r="B8" s="6">
-        <v>15</v>
-      </c>
-      <c r="C8" s="6">
-        <v>0.97194899700000004</v>
-      </c>
-      <c r="D8" s="9">
-        <v>5</v>
-      </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>0.91261479999999995</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="9">
         <v>4</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="9">
         <v>0.89734499999999995</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="11">
         <v>6</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="11">
         <v>0.94726399999999999</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="6">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5">
         <v>9</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0.94240409999999997</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="7">
         <v>2</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>0.83704849999999997</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="9">
         <v>3</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="9">
         <v>0.8599755</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H9" s="11">
         <v>4</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="11">
         <v>0.91111702000000006</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="5">
+        <v>25</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.98199672299999996</v>
+      </c>
+      <c r="D10" s="7">
         <v>7</v>
       </c>
-      <c r="B10" s="6">
-        <v>25</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0.98199672299999996</v>
-      </c>
-      <c r="D10" s="9">
+      <c r="E10" s="7">
+        <v>0.94469440000000005</v>
+      </c>
+      <c r="F10" s="9">
         <v>7</v>
       </c>
-      <c r="E10" s="9">
-        <v>0.94469440000000005</v>
-      </c>
-      <c r="F10" s="12">
-        <v>7</v>
-      </c>
-      <c r="G10" s="12">
+      <c r="G10" s="9">
         <v>0.95042899999999997</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="11">
         <v>11</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="11">
         <v>0.96119986000000002</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5">
+        <v>23</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.97507823900000001</v>
+      </c>
+      <c r="D11" s="7">
+        <v>9</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.95246920000000002</v>
+      </c>
+      <c r="F11" s="9">
         <v>8</v>
       </c>
-      <c r="B11" s="6">
-        <v>23</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0.97507823900000001</v>
-      </c>
-      <c r="D11" s="9">
-        <v>9</v>
-      </c>
-      <c r="E11" s="9">
-        <v>0.95246920000000002</v>
-      </c>
-      <c r="F11" s="12">
-        <v>8</v>
-      </c>
-      <c r="G11" s="12">
+      <c r="G11" s="9">
         <v>0.93827970000000005</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="11">
         <v>6</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="11">
         <v>0.90994889999999995</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="6">
+        <v>8</v>
+      </c>
+      <c r="B12" s="5">
         <v>2</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>0.86271717199999998</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="7">
         <v>1</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>0.8246945</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="9">
         <v>3</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="9">
         <v>0.94734496000000001</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="11">
         <v>1</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="11">
         <v>0.78387099999999998</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="6">
+        <v>9</v>
+      </c>
+      <c r="B13" s="5">
         <v>3</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>0.873</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="7">
         <v>1</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="7">
         <v>0.7070959</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="9">
         <v>1</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="9">
         <v>0.71739529999999996</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="11">
         <v>1</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="11">
         <v>0.81304759999999998</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="6">
+        <v>10</v>
+      </c>
+      <c r="B14" s="5">
         <v>6</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>0.95031019999999999</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="7">
         <v>3</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>0.87948999999999999</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="9">
         <v>1</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="9">
         <v>0.6847143</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="11">
         <v>2</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="11">
         <v>0.90616350000000001</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="6">
+        <v>11</v>
+      </c>
+      <c r="B15" s="5">
         <v>15</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>0.97210111700000001</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="7">
         <v>5</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>0.92711209999999999</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="9">
         <v>5</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="9">
         <v>0.92191440000000002</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="11">
         <v>5</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="11">
         <v>0.9214002</v>
       </c>
     </row>
@@ -1548,8 +1577,8 @@
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>